<commit_message>
for SemesterGradesSheet add MyStudents support
</commit_message>
<xml_diff>
--- a/AppData/Reports/GroupProgressSheet/Template.xlsx
+++ b/AppData/Reports/GroupProgressSheet/Template.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
-  <si>
-    <t>Итоговые оценки и зачеты за I семестр</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
   <si>
     <t>Средний балл</t>
   </si>
@@ -148,14 +145,173 @@
     <t>ДВИЖЕНИЕ ЧИСЛЕННОСТИ УЧАЩИХСЯ ЗА ИСТЕКШИЙ СЕМЕСТР (учебного года)</t>
   </si>
   <si>
-    <t>Число учащихся на начало учебного года dsfsdfsd sdfsdfsd sdfsdfsdf sdfsdf sdfsdfs sdfsdf</t>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Число учащихся на начало учебного года</t>
+  </si>
+  <si>
+    <t>Прибыло в течение семестра (учебного года) всего</t>
+  </si>
+  <si>
+    <t>ВЫБЫЛО УЧАЩИХСЯ ЗА СЕМЕСТР (учебного года) ВСЕГО   –  
+ИЗ НИХ:</t>
+  </si>
+  <si>
+    <t>Переведено с заочного обучения на дневное</t>
+  </si>
+  <si>
+    <t>Переведено из других техникумов</t>
+  </si>
+  <si>
+    <t>Восстановлено после демобилизации из состава Советской Армии</t>
+  </si>
+  <si>
+    <t>Вышло из академического отпуска</t>
+  </si>
+  <si>
+    <t>ИЗ НИХ:</t>
+  </si>
+  <si>
+    <t>по неуспеваемости</t>
+  </si>
+  <si>
+    <t>за нарушение дисциплины</t>
+  </si>
+  <si>
+    <t>переведено на заочное отделение</t>
+  </si>
+  <si>
+    <t>переведено в другие специальные учебные заведения</t>
+  </si>
+  <si>
+    <t>направлено на действительную службу в Советскую Армию</t>
+  </si>
+  <si>
+    <t>по семейным обстоятельствам</t>
+  </si>
+  <si>
+    <t>ушло в академический отпуск</t>
+  </si>
+  <si>
+    <t>ИТОГИ СЕМЕСТРОВЫХ И ПЕРЕВОДНЫХ ЭКЗАМЕНОВ</t>
+  </si>
+  <si>
+    <t>Численность учащихся к началу семестровых и переводных экзаменов</t>
+  </si>
+  <si>
+    <t>Явилось на экзамены</t>
+  </si>
+  <si>
+    <t>в том числе сдали экзамены и зачеты по всем предметам учебного плана</t>
+  </si>
+  <si>
+    <t>не ниже «8-9»</t>
+  </si>
+  <si>
+    <t>не ниже «6-7»</t>
+  </si>
+  <si>
+    <t>имели неудовлетворительную оценку по 1-2 предметам</t>
+  </si>
+  <si>
+    <t>имели неудовлетворительную оценку по трем и более предметам</t>
+  </si>
+  <si>
+    <t>Успеваемость в группе</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>Куратор группы</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">                     </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> Аргер Н.В. </t>
+    </r>
+  </si>
+  <si>
+    <t>Итоговые оценки и зачеты за 3 семестр</t>
+  </si>
+  <si>
+    <t>!-</t>
+  </si>
+  <si>
+    <t>!3</t>
+  </si>
+  <si>
+    <t>!12</t>
+  </si>
+  <si>
+    <t>Семестр 1 - 5</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">СВОДНАЯ ВЕДОМОСТЬ
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="204"/>
+      </rPr>
+      <t>успеваемости учащихся 2 курса, группы Т291-19
+за 3 семестр 2020/2021 учебного года</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,14 +335,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -223,6 +371,30 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -468,27 +640,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -506,13 +678,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -524,46 +696,46 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -572,13 +744,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -593,62 +762,85 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+      <selection activeCell="Z6" sqref="Z6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,127 +1140,153 @@
     <col min="25" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47"/>
-      <c r="B1" s="49" t="s">
+    <row r="1" spans="1:24" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50"/>
+      <c r="B1" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="49"/>
+      <c r="E1" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="T1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="V1" s="45"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="1:24" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="51" t="s">
+      <c r="E2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="J2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="55"/>
+      <c r="T2" s="43"/>
+      <c r="U2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="W2" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="40">
         <v>1</v>
       </c>
-      <c r="U1" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="V1" s="55"/>
-      <c r="W1" s="56"/>
-      <c r="X1" s="2"/>
-    </row>
-    <row r="2" spans="1:24" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="50"/>
-      <c r="C2" s="33" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="34"/>
-      <c r="P2" s="34"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="35"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="21" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="V2" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="2"/>
-    </row>
-    <row r="3" spans="1:24" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="41">
-        <v>1</v>
-      </c>
-      <c r="B3" s="42" t="s">
-        <v>3</v>
-      </c>
       <c r="C3" s="24">
         <v>6</v>
       </c>
-      <c r="D3" s="38">
-        <v>8</v>
-      </c>
-      <c r="E3" s="38">
+      <c r="D3" s="37">
+        <v>8</v>
+      </c>
+      <c r="E3" s="37">
         <v>10</v>
       </c>
-      <c r="F3" s="38">
-        <v>6</v>
-      </c>
-      <c r="G3" s="38">
-        <v>5</v>
-      </c>
-      <c r="H3" s="38">
+      <c r="F3" s="37">
+        <v>6</v>
+      </c>
+      <c r="G3" s="37">
+        <v>5</v>
+      </c>
+      <c r="H3" s="37">
         <v>7</v>
       </c>
-      <c r="I3" s="38">
-        <v>5</v>
-      </c>
-      <c r="J3" s="38">
+      <c r="I3" s="37">
+        <v>5</v>
+      </c>
+      <c r="J3" s="37">
         <v>7</v>
       </c>
-      <c r="K3" s="38">
-        <v>9</v>
-      </c>
-      <c r="L3" s="38">
-        <v>9</v>
-      </c>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
-      <c r="O3" s="38"/>
-      <c r="P3" s="38"/>
-      <c r="Q3" s="38"/>
+      <c r="K3" s="37">
+        <v>9</v>
+      </c>
+      <c r="L3" s="37">
+        <v>9</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
       <c r="R3" s="25"/>
       <c r="S3" s="24" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T3" s="25">
         <v>7.2</v>
@@ -1088,8 +1306,8 @@
       <c r="A4" s="14">
         <v>2</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>5</v>
+      <c r="B4" s="35" t="s">
+        <v>4</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -1098,7 +1316,7 @@
         <v>5</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="6">
         <v>4</v>
@@ -1128,7 +1346,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="26"/>
       <c r="S4" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T4" s="26">
         <v>4.8899999999999997</v>
@@ -1148,8 +1366,8 @@
       <c r="A5" s="14">
         <v>3</v>
       </c>
-      <c r="B5" s="36" t="s">
-        <v>7</v>
+      <c r="B5" s="35" t="s">
+        <v>6</v>
       </c>
       <c r="C5" s="14">
         <v>4</v>
@@ -1188,7 +1406,7 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="26"/>
       <c r="S5" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T5" s="26">
         <v>5.7</v>
@@ -1208,8 +1426,8 @@
       <c r="A6" s="14">
         <v>4</v>
       </c>
-      <c r="B6" s="36" t="s">
-        <v>8</v>
+      <c r="B6" s="35" t="s">
+        <v>7</v>
       </c>
       <c r="C6" s="14">
         <v>6</v>
@@ -1248,7 +1466,7 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="26"/>
       <c r="S6" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T6" s="26">
         <v>7.2</v>
@@ -1268,8 +1486,8 @@
       <c r="A7" s="14">
         <v>5</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>9</v>
+      <c r="B7" s="35" t="s">
+        <v>8</v>
       </c>
       <c r="C7" s="14">
         <v>5</v>
@@ -1308,7 +1526,7 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="26"/>
       <c r="S7" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T7" s="26">
         <v>6.4</v>
@@ -1328,8 +1546,8 @@
       <c r="A8" s="14">
         <v>6</v>
       </c>
-      <c r="B8" s="36" t="s">
-        <v>10</v>
+      <c r="B8" s="35" t="s">
+        <v>9</v>
       </c>
       <c r="C8" s="14">
         <v>9</v>
@@ -1368,7 +1586,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="26"/>
       <c r="S8" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T8" s="26">
         <v>8.3000000000000007</v>
@@ -1388,8 +1606,8 @@
       <c r="A9" s="14">
         <v>7</v>
       </c>
-      <c r="B9" s="36" t="s">
-        <v>11</v>
+      <c r="B9" s="35" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="14">
         <v>4</v>
@@ -1398,7 +1616,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="6">
         <v>4</v>
@@ -1428,7 +1646,7 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="26"/>
       <c r="S9" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T9" s="26">
         <v>4.5599999999999996</v>
@@ -1448,8 +1666,8 @@
       <c r="A10" s="14">
         <v>8</v>
       </c>
-      <c r="B10" s="36" t="s">
-        <v>12</v>
+      <c r="B10" s="35" t="s">
+        <v>11</v>
       </c>
       <c r="C10" s="14">
         <v>9</v>
@@ -1488,7 +1706,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="26"/>
       <c r="S10" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T10" s="26">
         <v>8.3000000000000007</v>
@@ -1508,8 +1726,8 @@
       <c r="A11" s="14">
         <v>9</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>13</v>
+      <c r="B11" s="35" t="s">
+        <v>12</v>
       </c>
       <c r="C11" s="14">
         <v>9</v>
@@ -1548,7 +1766,7 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="26"/>
       <c r="S11" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T11" s="26">
         <v>8.9</v>
@@ -1568,8 +1786,8 @@
       <c r="A12" s="14">
         <v>10</v>
       </c>
-      <c r="B12" s="36" t="s">
-        <v>14</v>
+      <c r="B12" s="35" t="s">
+        <v>13</v>
       </c>
       <c r="C12" s="14">
         <v>9</v>
@@ -1608,7 +1826,7 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="26"/>
       <c r="S12" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T12" s="26">
         <v>8.8000000000000007</v>
@@ -1628,8 +1846,8 @@
       <c r="A13" s="14">
         <v>11</v>
       </c>
-      <c r="B13" s="36" t="s">
-        <v>15</v>
+      <c r="B13" s="35" t="s">
+        <v>14</v>
       </c>
       <c r="C13" s="14">
         <v>5</v>
@@ -1668,7 +1886,7 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="26"/>
       <c r="S13" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T13" s="26">
         <v>6.3</v>
@@ -1688,8 +1906,8 @@
       <c r="A14" s="14">
         <v>12</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>16</v>
+      <c r="B14" s="35" t="s">
+        <v>15</v>
       </c>
       <c r="C14" s="14">
         <v>9</v>
@@ -1698,7 +1916,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="6">
         <v>9</v>
@@ -1728,7 +1946,7 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="26"/>
       <c r="S14" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T14" s="26">
         <v>8.89</v>
@@ -1748,8 +1966,8 @@
       <c r="A15" s="14">
         <v>13</v>
       </c>
-      <c r="B15" s="36" t="s">
-        <v>17</v>
+      <c r="B15" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="C15" s="14">
         <v>7</v>
@@ -1788,7 +2006,7 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="26"/>
       <c r="S15" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T15" s="26">
         <v>8.1999999999999993</v>
@@ -1808,8 +2026,8 @@
       <c r="A16" s="14">
         <v>14</v>
       </c>
-      <c r="B16" s="36" t="s">
-        <v>18</v>
+      <c r="B16" s="35" t="s">
+        <v>17</v>
       </c>
       <c r="C16" s="14">
         <v>6</v>
@@ -1848,7 +2066,7 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="26"/>
       <c r="S16" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T16" s="26">
         <v>6.3</v>
@@ -1868,8 +2086,8 @@
       <c r="A17" s="14">
         <v>15</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>19</v>
+      <c r="B17" s="35" t="s">
+        <v>18</v>
       </c>
       <c r="C17" s="14">
         <v>5</v>
@@ -1908,7 +2126,7 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="26"/>
       <c r="S17" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T17" s="26">
         <v>6.5</v>
@@ -1928,8 +2146,8 @@
       <c r="A18" s="14">
         <v>16</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>20</v>
+      <c r="B18" s="35" t="s">
+        <v>19</v>
       </c>
       <c r="C18" s="14">
         <v>4</v>
@@ -1968,7 +2186,7 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="26"/>
       <c r="S18" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T18" s="26">
         <v>6.6</v>
@@ -1988,8 +2206,8 @@
       <c r="A19" s="14">
         <v>17</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>21</v>
+      <c r="B19" s="35" t="s">
+        <v>20</v>
       </c>
       <c r="C19" s="14">
         <v>6</v>
@@ -2028,7 +2246,7 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="26"/>
       <c r="S19" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T19" s="26">
         <v>7.2</v>
@@ -2048,8 +2266,8 @@
       <c r="A20" s="14">
         <v>18</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>22</v>
+      <c r="B20" s="35" t="s">
+        <v>21</v>
       </c>
       <c r="C20" s="14">
         <v>8</v>
@@ -2088,7 +2306,7 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="26"/>
       <c r="S20" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T20" s="26">
         <v>8.1999999999999993</v>
@@ -2108,8 +2326,8 @@
       <c r="A21" s="14">
         <v>19</v>
       </c>
-      <c r="B21" s="36" t="s">
-        <v>23</v>
+      <c r="B21" s="35" t="s">
+        <v>22</v>
       </c>
       <c r="C21" s="14">
         <v>8</v>
@@ -2118,7 +2336,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F21" s="6">
         <v>8</v>
@@ -2148,7 +2366,7 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="26"/>
       <c r="S21" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T21" s="26">
         <v>8.2200000000000006</v>
@@ -2168,8 +2386,8 @@
       <c r="A22" s="14">
         <v>20</v>
       </c>
-      <c r="B22" s="36" t="s">
-        <v>24</v>
+      <c r="B22" s="35" t="s">
+        <v>23</v>
       </c>
       <c r="C22" s="14">
         <v>9</v>
@@ -2178,7 +2396,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="6">
         <v>8</v>
@@ -2208,7 +2426,7 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="26"/>
       <c r="S22" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T22" s="26">
         <v>8.11</v>
@@ -2228,8 +2446,8 @@
       <c r="A23" s="14">
         <v>21</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>25</v>
+      <c r="B23" s="35" t="s">
+        <v>24</v>
       </c>
       <c r="C23" s="14">
         <v>9</v>
@@ -2266,9 +2484,9 @@
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
-      <c r="R23" s="39"/>
+      <c r="R23" s="38"/>
       <c r="S23" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T23" s="26">
         <v>8.4</v>
@@ -2288,8 +2506,8 @@
       <c r="A24" s="14">
         <v>22</v>
       </c>
-      <c r="B24" s="36" t="s">
-        <v>26</v>
+      <c r="B24" s="35" t="s">
+        <v>25</v>
       </c>
       <c r="C24" s="14">
         <v>5</v>
@@ -2326,9 +2544,9 @@
       <c r="O24" s="9"/>
       <c r="P24" s="9"/>
       <c r="Q24" s="9"/>
-      <c r="R24" s="39"/>
+      <c r="R24" s="38"/>
       <c r="S24" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T24" s="26">
         <v>6.8</v>
@@ -2348,8 +2566,8 @@
       <c r="A25" s="14">
         <v>23</v>
       </c>
-      <c r="B25" s="36" t="s">
-        <v>27</v>
+      <c r="B25" s="35" t="s">
+        <v>26</v>
       </c>
       <c r="C25" s="14">
         <v>6</v>
@@ -2386,9 +2604,9 @@
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
       <c r="Q25" s="9"/>
-      <c r="R25" s="39"/>
+      <c r="R25" s="38"/>
       <c r="S25" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T25" s="26">
         <v>6.3</v>
@@ -2408,8 +2626,8 @@
       <c r="A26" s="16">
         <v>24</v>
       </c>
-      <c r="B26" s="37" t="s">
-        <v>28</v>
+      <c r="B26" s="36" t="s">
+        <v>27</v>
       </c>
       <c r="C26" s="16">
         <v>5</v>
@@ -2418,7 +2636,7 @@
         <v>5</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" s="17">
         <v>6</v>
@@ -2446,9 +2664,9 @@
       <c r="O26" s="18"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
-      <c r="R26" s="40"/>
+      <c r="R26" s="39"/>
       <c r="S26" s="16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T26" s="27">
         <v>5.78</v>
@@ -2483,7 +2701,7 @@
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
       <c r="S27" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="T27" s="12">
         <v>7.17</v>
@@ -2552,6 +2770,11 @@
       <c r="X29" s="2"/>
     </row>
     <row r="30" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="T1:T2"/>
@@ -2569,59 +2792,282 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:E20"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="5" max="5" width="60.5703125" customWidth="1"/>
+    <col min="1" max="1" width="60" style="58" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" style="60" customWidth="1"/>
+    <col min="3" max="3" width="13" style="57" customWidth="1"/>
+    <col min="4" max="4" width="55.28515625" style="57" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="57"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+    <row r="1" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="59" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="64"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="58"/>
-    </row>
-    <row r="5" spans="1:5" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="59">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="57"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="57"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="57"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="57"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="57"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E20" s="57"/>
+      <c r="C3" s="64"/>
+    </row>
+    <row r="4" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="61"/>
+      <c r="C4" s="64"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="63"/>
+      <c r="C5" s="64"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="63"/>
+      <c r="C6" s="64"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="63"/>
+      <c r="C7" s="64"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="63"/>
+      <c r="C8" s="64"/>
+    </row>
+    <row r="9" spans="1:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="56" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="64"/>
+      <c r="D10" s="56"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="64"/>
+      <c r="D11" s="56"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="64"/>
+      <c r="D12" s="56"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="64"/>
+      <c r="D13" s="56"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="64"/>
+      <c r="D14" s="56"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="64"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="63" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="64"/>
+    </row>
+    <row r="17" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="61"/>
+      <c r="C17" s="64"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="65" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="64"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="64"/>
+    </row>
+    <row r="20" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="64"/>
+    </row>
+    <row r="21" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="61"/>
+      <c r="C21" s="64"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="65" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="64"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="64"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="65" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="64"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="64"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="66">
+        <v>1</v>
+      </c>
+      <c r="C26" s="64"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="67"/>
+      <c r="B27" s="63"/>
+      <c r="C27" s="64"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="68" t="s">
+        <v>65</v>
+      </c>
+      <c r="B28" s="63"/>
+      <c r="C28" s="64"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="67"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="64"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="67"/>
+      <c r="B30" s="63"/>
+      <c r="C30" s="64"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="67"/>
+      <c r="B31" s="63"/>
+      <c r="C31" s="64"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="E15:E20"/>
+  <mergeCells count="6">
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A17:B17"/>
   </mergeCells>
-  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0.31496062992125984"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>